<commit_message>
[ODN-22] correct 1in diameters
</commit_message>
<xml_diff>
--- a/Tasks/ODN-22/ODN-22.xlsx
+++ b/Tasks/ODN-22/ODN-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\opticsdotnet\Tasks\ODN-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D96F40F-90D2-42AF-8CCB-2D33CFF9D2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B020A675-2677-4EBF-80AB-1C74EDC67434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{CB0C0625-BF89-43DB-88C3-E3E53FDDC7E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{CB0C0625-BF89-43DB-88C3-E3E53FDDC7E5}"/>
   </bookViews>
   <sheets>
     <sheet name="1in" sheetId="1" r:id="rId1"/>
@@ -812,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A273E92D-A006-4804-89D8-BEB40C5EC2F8}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,7 +866,7 @@
         <v>23</v>
       </c>
       <c r="P1">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q1" t="s">
         <v>23</v>
@@ -923,7 +923,7 @@
         <v>23</v>
       </c>
       <c r="P2">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q2" t="s">
         <v>23</v>
@@ -980,7 +980,7 @@
         <v>23</v>
       </c>
       <c r="P3">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q3" t="s">
         <v>23</v>
@@ -1037,7 +1037,7 @@
         <v>23</v>
       </c>
       <c r="P4">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q4" t="s">
         <v>23</v>
@@ -1094,7 +1094,7 @@
         <v>23</v>
       </c>
       <c r="P5">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q5" t="s">
         <v>23</v>
@@ -1151,7 +1151,7 @@
         <v>23</v>
       </c>
       <c r="P6">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q6" t="s">
         <v>23</v>
@@ -1208,7 +1208,7 @@
         <v>23</v>
       </c>
       <c r="P7">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q7" t="s">
         <v>23</v>
@@ -1265,7 +1265,7 @@
         <v>23</v>
       </c>
       <c r="P8">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -1322,7 +1322,7 @@
         <v>23</v>
       </c>
       <c r="P9">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -1379,7 +1379,7 @@
         <v>23</v>
       </c>
       <c r="P10">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
@@ -1436,7 +1436,7 @@
         <v>23</v>
       </c>
       <c r="P11">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q11" t="s">
         <v>23</v>
@@ -1493,7 +1493,7 @@
         <v>23</v>
       </c>
       <c r="P12">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q12" t="s">
         <v>23</v>
@@ -1550,7 +1550,7 @@
         <v>23</v>
       </c>
       <c r="P13">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q13" t="s">
         <v>23</v>
@@ -1607,7 +1607,7 @@
         <v>23</v>
       </c>
       <c r="P14">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q14" t="s">
         <v>23</v>
@@ -1664,7 +1664,7 @@
         <v>23</v>
       </c>
       <c r="P15">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q15" t="s">
         <v>23</v>
@@ -1721,7 +1721,7 @@
         <v>23</v>
       </c>
       <c r="P16">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q16" t="s">
         <v>23</v>
@@ -1778,7 +1778,7 @@
         <v>23</v>
       </c>
       <c r="P17">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q17" t="s">
         <v>23</v>
@@ -1835,7 +1835,7 @@
         <v>23</v>
       </c>
       <c r="P18">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q18" t="s">
         <v>23</v>
@@ -1892,7 +1892,7 @@
         <v>23</v>
       </c>
       <c r="P19">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q19" t="s">
         <v>23</v>
@@ -1949,7 +1949,7 @@
         <v>23</v>
       </c>
       <c r="P20">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q20" t="s">
         <v>23</v>
@@ -2006,7 +2006,7 @@
         <v>23</v>
       </c>
       <c r="P21">
-        <v>0.127</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q21" t="s">
         <v>23</v>
@@ -3667,7 +3667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E256BFFC-34D2-4523-9867-AB3A591F43F3}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[ODN-22] correct 30mm lenses
</commit_message>
<xml_diff>
--- a/Tasks/ODN-22/ODN-22.xlsx
+++ b/Tasks/ODN-22/ODN-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\opticsdotnet\Tasks\ODN-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B020A675-2677-4EBF-80AB-1C74EDC67434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFCF4A8-C122-4F7C-A179-67A8CBA21556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{CB0C0625-BF89-43DB-88C3-E3E53FDDC7E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{CB0C0625-BF89-43DB-88C3-E3E53FDDC7E5}"/>
   </bookViews>
   <sheets>
     <sheet name="1in" sheetId="1" r:id="rId1"/>
@@ -812,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A273E92D-A006-4804-89D8-BEB40C5EC2F8}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P1" sqref="P1:P21"/>
     </sheetView>
   </sheetViews>
@@ -2038,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C2A6B6-C973-400D-9A20-2F5270541A64}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="K1:S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2088,7 +2088,7 @@
         <v>23</v>
       </c>
       <c r="P1">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q1" t="s">
         <v>23</v>
@@ -2145,7 +2145,7 @@
         <v>23</v>
       </c>
       <c r="P2">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q2" t="s">
         <v>23</v>
@@ -2202,7 +2202,7 @@
         <v>23</v>
       </c>
       <c r="P3">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q3" t="s">
         <v>23</v>
@@ -2259,7 +2259,7 @@
         <v>23</v>
       </c>
       <c r="P4">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q4" t="s">
         <v>23</v>
@@ -2316,7 +2316,7 @@
         <v>23</v>
       </c>
       <c r="P5">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q5" t="s">
         <v>23</v>
@@ -2373,7 +2373,7 @@
         <v>23</v>
       </c>
       <c r="P6">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q6" t="s">
         <v>23</v>
@@ -2430,7 +2430,7 @@
         <v>23</v>
       </c>
       <c r="P7">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q7" t="s">
         <v>23</v>
@@ -2487,7 +2487,7 @@
         <v>23</v>
       </c>
       <c r="P8">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q8" t="s">
         <v>23</v>
@@ -2544,7 +2544,7 @@
         <v>23</v>
       </c>
       <c r="P9">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>

</xml_diff>